<commit_message>
Finalizado, falta la planificacion
</commit_message>
<xml_diff>
--- a/Sistemas para control/tablas parcial 1.xlsx
+++ b/Sistemas para control/tablas parcial 1.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema de memoria modbus" sheetId="1" r:id="rId1"/>
     <sheet name="presupuesto" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>Adress</t>
   </si>
@@ -181,6 +182,60 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Presupuesto estacion central</t>
+  </si>
+  <si>
+    <t>Presupuesto nodo</t>
+  </si>
+  <si>
+    <t>Cant</t>
+  </si>
+  <si>
+    <t>Anemometro Wallis &amp; Gill Ak3</t>
+  </si>
+  <si>
+    <t>Raspberry pi + case</t>
+  </si>
+  <si>
+    <t>Sensor temperatura ds18b20</t>
+  </si>
+  <si>
+    <t>Pantalla tactil 5 pulgadas</t>
+  </si>
+  <si>
+    <t>Electronica complementaria (conectores, cables)</t>
+  </si>
+  <si>
+    <t>Torre reticulada 20m de altura</t>
+  </si>
+  <si>
+    <t>Arduino UNO R3</t>
+  </si>
+  <si>
+    <t>Sensor temp y humedad SHT-30</t>
+  </si>
+  <si>
+    <t>Sensor humedad del suelo</t>
+  </si>
+  <si>
+    <t>Sensor ds18b20</t>
+  </si>
+  <si>
+    <t>Modulo LoRa 433MHz + antena 6dBi</t>
+  </si>
+  <si>
+    <t>Electronica complementaria (cables, conectores)</t>
+  </si>
+  <si>
+    <t>Panel solar 5V 1W</t>
+  </si>
+  <si>
+    <t>Powerbank 20000mAh</t>
+  </si>
+  <si>
+    <t>Gabinete</t>
   </si>
 </sst>
 </file>
@@ -190,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +254,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -339,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -364,6 +427,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -373,10 +440,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -660,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -967,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -980,15 +1046,15 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -997,27 +1063,27 @@
       <c r="D3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="11">
-        <v>160000</v>
+        <v>260000</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="14">
         <f t="shared" ref="E4:E14" si="0">C4*D4</f>
-        <v>320000</v>
+        <v>520000</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="11">
@@ -1026,13 +1092,13 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="11">
@@ -1041,13 +1107,13 @@
       <c r="D6" s="1">
         <v>6</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <f t="shared" si="0"/>
         <v>39000</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="11">
@@ -1056,13 +1122,13 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="11">
@@ -1071,13 +1137,13 @@
       <c r="D8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="11">
@@ -1086,13 +1152,13 @@
       <c r="D9" s="1">
         <v>2</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="11">
@@ -1101,13 +1167,13 @@
       <c r="D10" s="1">
         <v>4</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="11">
@@ -1116,13 +1182,13 @@
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="14">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="11">
@@ -1131,13 +1197,13 @@
       <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="14">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="11">
@@ -1146,13 +1212,13 @@
       <c r="D13" s="1">
         <v>10</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="11">
@@ -1161,13 +1227,13 @@
       <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="14">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="13" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="11">
@@ -1176,13 +1242,13 @@
       <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="14">
         <f>C15*D15</f>
         <v>13000</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="11">
@@ -1191,13 +1257,13 @@
       <c r="D16" s="1">
         <v>50</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="14">
         <f>C16*D16</f>
         <v>1650</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="11">
@@ -1206,13 +1272,13 @@
       <c r="D17" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="14">
         <f>C17*D17</f>
         <v>2400</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="11">
@@ -1221,13 +1287,13 @@
       <c r="D18" s="1">
         <v>40</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="14">
         <f>C18*D18</f>
         <v>2720</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="11">
@@ -1236,26 +1302,26 @@
       <c r="D19" s="1">
         <v>2</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="14">
         <f>C19*D19</f>
         <v>5200</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="16"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="17"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="18">
+      <c r="E21" s="15">
         <f>SUM(E4:E20)</f>
-        <v>428970</v>
+        <v>628970</v>
       </c>
     </row>
   </sheetData>
@@ -1264,4 +1330,369 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="40.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="7" max="7" width="40.7265625" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" customWidth="1"/>
+    <col min="9" max="9" width="4.6328125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="G2" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="11">
+        <v>14400</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" ref="E4:E9" si="0">C4*D4</f>
+        <v>14400</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" ref="J4:J9" si="1">H4*I4</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="11">
+        <v>9200</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" si="0"/>
+        <v>9200</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="11">
+        <v>930</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="1"/>
+        <v>930</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="11">
+        <v>200</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="11">
+        <v>540</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="1"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1500</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="11">
+        <v>200</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="11">
+        <v>9000</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="11">
+        <v>600</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="11">
+        <v>500</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="11">
+        <v>6500</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14">
+        <f>C10*D10</f>
+        <v>6500</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="11">
+        <v>725</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5</v>
+      </c>
+      <c r="J10" s="14">
+        <f>H10*I10</f>
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="11">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1">
+        <v>40</v>
+      </c>
+      <c r="E11" s="14">
+        <f>C11*D11</f>
+        <v>1320</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="11">
+        <v>2510</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="14">
+        <f>H11*I11</f>
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="11">
+        <v>68</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="14">
+        <f>C12*D12</f>
+        <v>680</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="11">
+        <v>3000</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="14">
+        <f>H12*I12</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="19">
+        <v>15000</v>
+      </c>
+      <c r="D13" s="20">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
+        <f>C13*D13</f>
+        <v>15000</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="15">
+        <f>SUM(E4:E13)</f>
+        <v>59200</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="15">
+        <f>SUM(J4:J13)</f>
+        <v>12905</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>